<commit_message>
added /time to src
</commit_message>
<xml_diff>
--- a/device_id.xlsx
+++ b/device_id.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\E-motion chair\E-motion chair v0.3.0\ontwikkeling\E-Motion-chair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC040E1F-8A91-42AB-85A5-8A2BAA39C0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F912881-802C-471A-8377-862872C3C815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="980" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="1" r:id="rId1"/>
-    <sheet name="EM-1521042" sheetId="5" r:id="rId2"/>
-    <sheet name="EM-1521142" sheetId="3" r:id="rId3"/>
-    <sheet name="EM-1521152" sheetId="4" r:id="rId4"/>
-    <sheet name="EM-1521400" sheetId="2" r:id="rId5"/>
+    <sheet name="EM-1521056" sheetId="6" r:id="rId2"/>
+    <sheet name="EM-1521042" sheetId="5" r:id="rId3"/>
+    <sheet name="EM-1521142" sheetId="3" r:id="rId4"/>
+    <sheet name="EM-1521152" sheetId="4" r:id="rId5"/>
+    <sheet name="EM-1521400" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t xml:space="preserve">Nummer op bat </t>
   </si>
@@ -201,6 +202,9 @@
   <si>
     <t xml:space="preserve">uren </t>
   </si>
+  <si>
+    <t>yes</t>
+  </si>
 </sst>
 </file>
 
@@ -259,7 +263,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -283,6 +287,15 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="2" builtinId="3"/>
@@ -1961,6 +1974,104 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>94400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>78700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Afbeelding 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFB47342-F012-4121-8760-8B39EB729B4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="3585882"/>
+          <a:ext cx="6800000" cy="2409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>8686</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>146369</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Afbeelding 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22027396-111C-411E-BB0C-32C4B04EEEC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3840480"/>
+          <a:ext cx="6714286" cy="2523809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
@@ -2006,7 +2117,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2055,7 +2166,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2361,8 +2472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2426,30 +2537,45 @@
       <c r="E3" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+      <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="14">
         <v>272911208406908</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="13">
         <v>400</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2478,6 +2604,9 @@
       <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
@@ -2504,6 +2633,9 @@
       <c r="I6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
@@ -2528,6 +2660,9 @@
         <v>6</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2537,11 +2672,414 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4944568-8180-434E-8DCB-DD967DA9B2F4}">
+  <dimension ref="B3:L18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>464</v>
+      </c>
+      <c r="E5">
+        <v>920</v>
+      </c>
+      <c r="G5">
+        <v>3181</v>
+      </c>
+      <c r="I5">
+        <v>4437</v>
+      </c>
+      <c r="K5">
+        <v>5408</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>272</v>
+      </c>
+      <c r="E6">
+        <v>925</v>
+      </c>
+      <c r="G6">
+        <v>2932</v>
+      </c>
+      <c r="I6">
+        <v>4469</v>
+      </c>
+      <c r="K6">
+        <v>5057</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>489</v>
+      </c>
+      <c r="E7">
+        <v>1232</v>
+      </c>
+      <c r="G7">
+        <v>3217</v>
+      </c>
+      <c r="I7">
+        <v>4621</v>
+      </c>
+      <c r="K7">
+        <v>5532</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>229</v>
+      </c>
+      <c r="E8">
+        <v>1085</v>
+      </c>
+      <c r="G8">
+        <v>2720</v>
+      </c>
+      <c r="I8">
+        <v>4045</v>
+      </c>
+      <c r="K8">
+        <v>5160</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>293</v>
+      </c>
+      <c r="E9">
+        <v>869</v>
+      </c>
+      <c r="G9">
+        <v>2465</v>
+      </c>
+      <c r="I9">
+        <v>3917</v>
+      </c>
+      <c r="K9">
+        <v>4924</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>561</v>
+      </c>
+      <c r="E10">
+        <v>1113</v>
+      </c>
+      <c r="G10">
+        <v>2552</v>
+      </c>
+      <c r="I10">
+        <v>4120</v>
+      </c>
+      <c r="K10">
+        <v>5105</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>216</v>
+      </c>
+      <c r="E11">
+        <v>753</v>
+      </c>
+      <c r="G11">
+        <v>2469</v>
+      </c>
+      <c r="I11">
+        <v>4133</v>
+      </c>
+      <c r="K11">
+        <v>5073</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>692</v>
+      </c>
+      <c r="E12">
+        <v>1260</v>
+      </c>
+      <c r="G12">
+        <v>2760</v>
+      </c>
+      <c r="I12">
+        <v>4345</v>
+      </c>
+      <c r="K12">
+        <v>4913</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>344</v>
+      </c>
+      <c r="E13">
+        <v>1144</v>
+      </c>
+      <c r="G13">
+        <v>2753</v>
+      </c>
+      <c r="I13">
+        <v>4004</v>
+      </c>
+      <c r="K13">
+        <v>5069</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="3">
+        <f>_xlfn.STDEV.S(C5:C13)</f>
+        <v>164.73092538372319</v>
+      </c>
+      <c r="D15" s="3" t="e">
+        <f t="shared" ref="D15:L15" si="0">_xlfn.STDEV.S(D5:D13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>174.02665823883925</v>
+      </c>
+      <c r="F15" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>280.05346711734251</v>
+      </c>
+      <c r="H15" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>242.59173522607895</v>
+      </c>
+      <c r="J15" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="0"/>
+        <v>206.66303760254544</v>
+      </c>
+      <c r="L15" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <f>MIN(C5:C13)</f>
+        <v>216</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:L16" si="1">MIN(D5:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>753</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>2465</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>3917</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>4913</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <f>MAX(C5:C13)</f>
+        <v>692</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:L17" si="2">MAX(D5:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>1260</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>3217</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>4621</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>5532</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <f>ABS(C16-C17)</f>
+        <v>476</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:L18" si="3">ABS(D16-D17)</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>507</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>752</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>704</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>619</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52BEE75-0815-45D3-AF06-324863A97F72}">
   <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2935,10 +3473,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA08E70E-6485-4B4B-B27A-0ADF0208C1DE}">
   <dimension ref="B2:L28"/>
   <sheetViews>
@@ -3434,11 +3973,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650D7530-4C62-4FDA-BEE1-FF52241A5947}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -3865,7 +4404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8063B206-5FA7-4448-8EF9-9594290099CF}">
   <dimension ref="C2:M75"/>
   <sheetViews>

</xml_diff>